<commit_message>
update notes and bugs
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,12 +14,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Student Grades:</t>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>math</t>
   </si>
   <si>
     <t>Student Average:</t>
+  </si>
+  <si>
+    <t>Average:</t>
   </si>
 </sst>
 </file>
@@ -351,7 +360,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -362,12 +371,33 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing bug average of students
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,21 +14,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+  <si>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
   <si>
     <t>Student</t>
   </si>
   <si>
-    <t>b</t>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>bb</t>
   </si>
   <si>
     <t>math</t>
   </si>
   <si>
-    <t>Student Average:</t>
+    <t>hist</t>
   </si>
   <si>
     <t>Average:</t>
+  </si>
+  <si>
+    <t>Students Average:</t>
+  </si>
+  <si>
+    <t>Median:</t>
+  </si>
+  <si>
+    <t>Excellent Students:</t>
   </si>
 </sst>
 </file>
@@ -360,44 +381,134 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>90</v>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>50.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>88.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18">
+        <v>69.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19">
+        <v>69.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>88.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>88.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add prints to program
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Teacher</t>
   </si>
@@ -22,25 +22,7 @@
     <t>a</t>
   </si>
   <si>
-    <t>b</t>
-  </si>
-  <si>
     <t>Student</t>
-  </si>
-  <si>
-    <t>aa</t>
-  </si>
-  <si>
-    <t>bb</t>
-  </si>
-  <si>
-    <t>math</t>
-  </si>
-  <si>
-    <t>hist</t>
-  </si>
-  <si>
-    <t>Average:</t>
   </si>
   <si>
     <t>Students Average:</t>
@@ -381,134 +363,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11">
-        <v>50.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
         <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="B15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15">
-        <v>88.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18">
-        <v>69.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19">
-        <v>69.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21">
-        <v>88.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" t="s">
-        <v>2</v>
-      </c>
-      <c r="C23">
-        <v>88.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>